<commit_message>
new: interface for upload files(.xls or .xlsx) and process data in the same time
</commit_message>
<xml_diff>
--- a/Endpoint/Endpoint/files/teste.xlsx
+++ b/Endpoint/Endpoint/files/teste.xlsx
@@ -8,15 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="Vendas" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="79">
+  <si>
+    <t>Número do Pedido</t>
+  </si>
   <si>
     <t>E-mail</t>
   </si>
@@ -48,6 +49,9 @@
     <t>Total</t>
   </si>
   <si>
+    <t>Nome do comprador</t>
+  </si>
+  <si>
     <t>CPF / CNPJ</t>
   </si>
   <si>
@@ -105,6 +109,9 @@
     <t>Data de envío</t>
   </si>
   <si>
+    <t>Nome do Produto</t>
+  </si>
+  <si>
     <t>Valor do Produto</t>
   </si>
   <si>
@@ -117,6 +124,15 @@
     <t>Canal</t>
   </si>
   <si>
+    <t>Identificador da transação no meio de pagamento</t>
+  </si>
+  <si>
+    <t>Identificador do pedido</t>
+  </si>
+  <si>
+    <t>Produto Fisico</t>
+  </si>
+  <si>
     <t>ana.c.dinda@hotmail.com</t>
   </si>
   <si>
@@ -135,6 +151,9 @@
     <t>Ana Claudia de Moura Silva</t>
   </si>
   <si>
+    <t>11 974557678</t>
+  </si>
+  <si>
     <t>Ana</t>
   </si>
   <si>
@@ -171,6 +190,12 @@
     <t>Mobile</t>
   </si>
   <si>
+    <t>FC62BCC3-F8CC-407C-BB0D-40BDCEAFA6E9</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
     <t>oliversmelissa@hotmail.com</t>
   </si>
   <si>
@@ -192,12 +217,18 @@
     <t>Loja virtual</t>
   </si>
   <si>
+    <t>658E3E6E-5330-4996-9EE7-1A78C4C182D0</t>
+  </si>
+  <si>
+    <t>Pendente</t>
+  </si>
+  <si>
+    <t>Correios - SEDEX (via Melhor Envio)</t>
+  </si>
+  <si>
     <t>medeirossclaudio@gmail.com</t>
   </si>
   <si>
-    <t>Pendente</t>
-  </si>
-  <si>
     <t>11.75</t>
   </si>
   <si>
@@ -207,9 +238,6 @@
     <t>Claudio Filho Téu</t>
   </si>
   <si>
-    <t>11 981568415</t>
-  </si>
-  <si>
     <t>Rua Itabira</t>
   </si>
   <si>
@@ -219,59 +247,17 @@
     <t>Jandira</t>
   </si>
   <si>
-    <t>Correios - SEDEX (via Melhor Envio)</t>
-  </si>
-  <si>
     <t>Caneca Magica  Mapa do Maroto</t>
   </si>
   <si>
-    <t>gabrielamartins767@gmail.com</t>
-  </si>
-  <si>
-    <t>16.8</t>
-  </si>
-  <si>
-    <t>157.8</t>
-  </si>
-  <si>
-    <t>Gabriela Santos</t>
-  </si>
-  <si>
-    <t>Gabriela</t>
-  </si>
-  <si>
-    <t>Rua Giovanni Nasco</t>
-  </si>
-  <si>
-    <t>Apt 44a</t>
-  </si>
-  <si>
-    <t>Conjunto Habitacional Teotonio Vilela</t>
-  </si>
-  <si>
-    <t>Número do Pedido</t>
-  </si>
-  <si>
-    <t>Nome do comprador</t>
-  </si>
-  <si>
-    <t>Nome do Produto</t>
-  </si>
-  <si>
-    <t>Identificador da transação no meio de pagamento</t>
-  </si>
-  <si>
-    <t>Identificador do pedido</t>
-  </si>
-  <si>
-    <t>Produto Fisico</t>
+    <t>9AA56999-D2D9-47D9-A964-BFABE392EFF4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,23 +266,316 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -304,17 +583,205 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Ênfase1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bom" xfId="19" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="20" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Célula de Verificação" xfId="21" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Célula Vinculada" xfId="22" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Ênfase1" xfId="23" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Ênfase2" xfId="24" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Ênfase3" xfId="25" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Ênfase4" xfId="26" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Ênfase5" xfId="27" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Ênfase6" xfId="28" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="29" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorreto" xfId="30" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutra" xfId="31" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Nota" xfId="32" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Saída" xfId="33" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de Aviso" xfId="34" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto Explicativo" xfId="35" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="36" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="37" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="38" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="39" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Título 4" xfId="40" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -606,135 +1073,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AN7"/>
+  <dimension ref="A1:AN4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="R1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="T1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="V1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Y1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AA1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="AB1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="AC1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AD1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AE1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="AF1" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="AG1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="AH1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="AI1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="AJ1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="AL1" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="AM1" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="AN1" t="s">
-        <v>82</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:40">
@@ -742,22 +1208,22 @@
         <v>198</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="2">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1">
         <v>44042</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="H2">
         <v>141</v>
@@ -772,58 +1238,58 @@
         <v>141</v>
       </c>
       <c r="L2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="M2">
         <v>49440609800</v>
       </c>
-      <c r="N2" t="s">
-        <v>63</v>
+      <c r="N2">
+        <v>11981568415</v>
       </c>
       <c r="O2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="P2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="Q2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="R2">
         <v>151</v>
       </c>
       <c r="S2" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="T2" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="U2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="V2">
         <v>6440175</v>
       </c>
       <c r="W2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="X2" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="Y2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="Z2" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="AA2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD2" s="2">
+        <v>55</v>
+      </c>
+      <c r="AD2" s="1">
         <v>44042</v>
       </c>
       <c r="AF2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="AG2">
         <v>47</v>
@@ -835,7 +1301,16 @@
         <v>3151</v>
       </c>
       <c r="AJ2" t="s">
-        <v>50</v>
+        <v>57</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM2">
+        <v>270849502</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:40">
@@ -843,22 +1318,22 @@
         <v>197</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="2">
+        <v>60</v>
+      </c>
+      <c r="C3" s="1">
         <v>44042</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="H3">
         <v>141</v>
@@ -873,7 +1348,7 @@
         <v>141</v>
       </c>
       <c r="L3" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="M3">
         <v>41810810876</v>
@@ -882,43 +1357,43 @@
         <v>11981568415</v>
       </c>
       <c r="O3" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="P3">
-        <v>11981568415</v>
+        <v>11988668126</v>
       </c>
       <c r="Q3" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="R3">
         <v>24</v>
       </c>
       <c r="T3" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="U3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="V3">
         <v>6454000</v>
       </c>
       <c r="W3" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="X3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="Y3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="Z3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="AA3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="AF3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="AG3">
         <v>47</v>
@@ -930,7 +1405,16 @@
         <v>3151</v>
       </c>
       <c r="AJ3" t="s">
-        <v>57</v>
+        <v>66</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM3">
+        <v>270669524</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:40">
@@ -938,22 +1422,22 @@
         <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="2">
+        <v>70</v>
+      </c>
+      <c r="C4" s="1">
         <v>44039</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="H4">
         <v>47</v>
@@ -962,13 +1446,13 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="K4" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="L4" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="M4">
         <v>38554442857</v>
@@ -977,40 +1461,40 @@
         <v>11981568415</v>
       </c>
       <c r="O4" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="P4">
-        <v>11981568415</v>
+        <v>11946783909</v>
       </c>
       <c r="Q4" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="R4">
         <v>62</v>
       </c>
       <c r="T4" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="U4" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="V4">
         <v>6620289</v>
       </c>
       <c r="W4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="X4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="Y4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Z4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="AF4" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="AG4">
         <v>47</v>
@@ -1022,133 +1506,19 @@
         <v>9</v>
       </c>
       <c r="AJ4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:40">
-      <c r="A5">
-        <v>174</v>
-      </c>
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="2">
-        <v>44039</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM4">
+        <v>268346090</v>
+      </c>
+      <c r="AN4" t="s">
         <v>59</v>
       </c>
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5">
-        <v>141</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>70</v>
-      </c>
-      <c r="K5" t="s">
-        <v>71</v>
-      </c>
-      <c r="L5" t="s">
-        <v>72</v>
-      </c>
-      <c r="M5">
-        <v>37771961851</v>
-      </c>
-      <c r="N5">
-        <v>11981568415</v>
-      </c>
-      <c r="O5" t="s">
-        <v>73</v>
-      </c>
-      <c r="P5">
-        <v>11981568415</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>74</v>
-      </c>
-      <c r="R5">
-        <v>55</v>
-      </c>
-      <c r="S5" t="s">
-        <v>75</v>
-      </c>
-      <c r="T5" t="s">
-        <v>76</v>
-      </c>
-      <c r="U5" t="s">
-        <v>44</v>
-      </c>
-      <c r="V5">
-        <v>3928090</v>
-      </c>
-      <c r="W5" t="s">
-        <v>44</v>
-      </c>
-      <c r="X5" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG5">
-        <v>47</v>
-      </c>
-      <c r="AH5">
-        <v>3</v>
-      </c>
-      <c r="AI5">
-        <v>9</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:40">
-      <c r="F7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new: add textbox on upload.aspx
</commit_message>
<xml_diff>
--- a/Endpoint/Endpoint/files/teste.xlsx
+++ b/Endpoint/Endpoint/files/teste.xlsx
@@ -148,15 +148,9 @@
     <t>BRL</t>
   </si>
   <si>
-    <t>Ana Claudia de Moura Silva</t>
-  </si>
-  <si>
     <t>11 974557678</t>
   </si>
   <si>
-    <t>Ana</t>
-  </si>
-  <si>
     <t>Avenida Marginal Esquerda</t>
   </si>
   <si>
@@ -251,6 +245,12 @@
   </si>
   <si>
     <t>9AA56999-D2D9-47D9-A964-BFABE392EFF4</t>
+  </si>
+  <si>
+    <t>Sara Alcaras</t>
+  </si>
+  <si>
+    <t>Caneca lol nami</t>
   </si>
 </sst>
 </file>
@@ -1075,13 +1075,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="53.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40">
@@ -1238,58 +1239,58 @@
         <v>141</v>
       </c>
       <c r="L2" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="M2">
         <v>49440609800</v>
       </c>
       <c r="N2">
-        <v>11981568415</v>
+        <v>11997035927</v>
       </c>
       <c r="O2" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="P2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q2" t="s">
         <v>45</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>47</v>
       </c>
       <c r="R2">
         <v>151</v>
       </c>
       <c r="S2" t="s">
+        <v>46</v>
+      </c>
+      <c r="T2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" t="s">
         <v>48</v>
-      </c>
-      <c r="T2" t="s">
-        <v>49</v>
-      </c>
-      <c r="U2" t="s">
-        <v>50</v>
       </c>
       <c r="V2">
         <v>6440175</v>
       </c>
       <c r="W2" t="s">
+        <v>49</v>
+      </c>
+      <c r="X2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y2" t="s">
         <v>51</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>52</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>53</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>55</v>
       </c>
       <c r="AD2" s="1">
         <v>44042</v>
       </c>
       <c r="AF2" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="AG2">
         <v>47</v>
@@ -1301,16 +1302,16 @@
         <v>3151</v>
       </c>
       <c r="AJ2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AL2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AM2">
         <v>270849502</v>
       </c>
       <c r="AN2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:40">
@@ -1318,16 +1319,16 @@
         <v>197</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1">
         <v>44042</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F3" t="s">
         <v>42</v>
@@ -1348,7 +1349,7 @@
         <v>141</v>
       </c>
       <c r="L3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="M3">
         <v>41810810876</v>
@@ -1357,43 +1358,43 @@
         <v>11981568415</v>
       </c>
       <c r="O3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P3">
         <v>11988668126</v>
       </c>
       <c r="Q3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R3">
         <v>24</v>
       </c>
       <c r="T3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="U3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="V3">
         <v>6454000</v>
       </c>
       <c r="W3" t="s">
+        <v>49</v>
+      </c>
+      <c r="X3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y3" t="s">
         <v>51</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Z3" t="s">
         <v>52</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AA3" t="s">
         <v>53</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AF3" t="s">
         <v>54</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>56</v>
       </c>
       <c r="AG3">
         <v>47</v>
@@ -1405,16 +1406,16 @@
         <v>3151</v>
       </c>
       <c r="AJ3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AL3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AM3">
         <v>270669524</v>
       </c>
       <c r="AN3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:40">
@@ -1422,16 +1423,16 @@
         <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" s="1">
         <v>44039</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F4" t="s">
         <v>42</v>
@@ -1446,13 +1447,13 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L4" t="s">
         <v>71</v>
-      </c>
-      <c r="K4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L4" t="s">
-        <v>73</v>
       </c>
       <c r="M4">
         <v>38554442857</v>
@@ -1461,40 +1462,40 @@
         <v>11981568415</v>
       </c>
       <c r="O4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P4">
         <v>11946783909</v>
       </c>
       <c r="Q4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="R4">
         <v>62</v>
       </c>
       <c r="T4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="U4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="V4">
         <v>6620289</v>
       </c>
       <c r="W4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="X4" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z4" t="s">
         <v>52</v>
       </c>
-      <c r="Y4" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>54</v>
-      </c>
       <c r="AF4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AG4">
         <v>47</v>
@@ -1506,16 +1507,16 @@
         <v>9</v>
       </c>
       <c r="AJ4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AL4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AM4">
         <v>268346090</v>
       </c>
       <c r="AN4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>